<commit_message>
marble madness - lv 1 done, 8 frames faster
</commit_message>
<xml_diff>
--- a/GenesisMarbleMadness/FrameCompare.xlsx
+++ b/GenesisMarbleMadness/FrameCompare.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\GenesisMarbleMadness\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB7F6038-0E1D-44CD-AA7B-F6F44BC6356C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08E1E183-C614-4AB1-9ADB-7189D0B5F51C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="177">
   <si>
     <t>Place</t>
   </si>
@@ -556,6 +556,15 @@
   </si>
   <si>
     <t>1st Move</t>
+  </si>
+  <si>
+    <t>Goal</t>
+  </si>
+  <si>
+    <t>Fadeout</t>
+  </si>
+  <si>
+    <t>Lv 2 Appears</t>
   </si>
 </sst>
 </file>
@@ -1343,7 +1352,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1372,34 +1381,46 @@
       <c r="A2" s="42" t="s">
         <v>168</v>
       </c>
-      <c r="B2" s="2"/>
+      <c r="B2" s="2">
+        <v>181</v>
+      </c>
       <c r="C2" s="2">
         <v>180</v>
       </c>
-      <c r="D2" s="3" t="str">
+      <c r="D2" s="3">
         <f>IF(C2&lt;&gt;"",IF(B2&lt;&gt;"",C2-B2,"-"), "-")</f>
-        <v>-</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="42" t="s">
         <v>169</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2">
+        <v>294</v>
+      </c>
       <c r="C3" s="2">
         <v>291</v>
       </c>
-      <c r="D3" s="3"/>
+      <c r="D3" s="3">
+        <f>IF(C3&lt;&gt;"",IF(B3&lt;&gt;"",C3-B3,"-"), "-")</f>
+        <v>-3</v>
+      </c>
     </row>
     <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="42" t="s">
         <v>170</v>
       </c>
-      <c r="B4" s="2"/>
+      <c r="B4" s="2">
+        <v>405</v>
+      </c>
       <c r="C4" s="2">
         <v>422</v>
       </c>
-      <c r="D4" s="3"/>
+      <c r="D4" s="3">
+        <f t="shared" ref="D4:D16" si="0">IF(C4&lt;&gt;"",IF(B4&lt;&gt;"",C4-B4,"-"), "-")</f>
+        <v>17</v>
+      </c>
       <c r="E4" t="s">
         <v>171</v>
       </c>
@@ -1408,51 +1429,92 @@
       <c r="A5" s="42" t="s">
         <v>172</v>
       </c>
-      <c r="B5" s="2"/>
+      <c r="B5" s="2">
+        <v>526</v>
+      </c>
       <c r="C5" s="2">
         <v>542</v>
       </c>
-      <c r="D5" s="3"/>
+      <c r="D5" s="3">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
     </row>
     <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="42" t="s">
         <v>173</v>
       </c>
-      <c r="B6" s="2"/>
+      <c r="B6" s="2">
+        <v>736</v>
+      </c>
       <c r="C6" s="2">
         <v>749</v>
       </c>
-      <c r="D6" s="3"/>
+      <c r="D6" s="3">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
     </row>
     <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="42"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="3"/>
+      <c r="A7" s="42" t="s">
+        <v>174</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1101</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1107</v>
+      </c>
+      <c r="D7" s="3">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
     </row>
     <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="42"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="3"/>
+      <c r="A8" s="42" t="s">
+        <v>175</v>
+      </c>
+      <c r="B8" s="2">
+        <v>1316</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1341</v>
+      </c>
+      <c r="D8" s="3">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
     </row>
     <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="42"/>
+      <c r="A9" s="42" t="s">
+        <v>176</v>
+      </c>
       <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="3"/>
+      <c r="C9" s="2">
+        <v>1462</v>
+      </c>
+      <c r="D9" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="42"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
-      <c r="D10" s="3"/>
+      <c r="D10" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="33"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
-      <c r="D11" s="3"/>
+      <c r="D11" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="42" t="s">
@@ -1462,7 +1524,10 @@
       <c r="C12" s="2">
         <v>7928</v>
       </c>
-      <c r="D12" s="3"/>
+      <c r="D12" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
@@ -1473,7 +1538,7 @@
         <v>9567</v>
       </c>
       <c r="D13" s="3" t="str">
-        <f>IF(C13&lt;&gt;"",IF(B13&lt;&gt;"",C13-B13,"-"), "-")</f>
+        <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
@@ -1482,7 +1547,7 @@
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
       <c r="D14" s="3" t="str">
-        <f>IF(C14&lt;&gt;"",IF(B14&lt;&gt;"",C14-B14,"-"), "-")</f>
+        <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
@@ -1491,7 +1556,7 @@
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
       <c r="D15" s="3" t="str">
-        <f>IF(C15&lt;&gt;"",IF(B15&lt;&gt;"",C15-B15,"-"), "-")</f>
+        <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
@@ -1500,7 +1565,7 @@
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
       <c r="D16" s="3" t="str">
-        <f>IF(C16&lt;&gt;"",IF(B16&lt;&gt;"",C16-B16,"-"), "-")</f>
+        <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
@@ -1761,7 +1826,7 @@
       <c r="B45" s="7"/>
       <c r="C45" s="7"/>
       <c r="D45" s="3" t="str">
-        <f t="shared" ref="D45:D49" si="0">IF(C45&lt;&gt;"",IF(B45&lt;&gt;"",C45-B45,"-"), "-")</f>
+        <f t="shared" ref="D45:D49" si="1">IF(C45&lt;&gt;"",IF(B45&lt;&gt;"",C45-B45,"-"), "-")</f>
         <v>-</v>
       </c>
     </row>
@@ -1770,7 +1835,7 @@
       <c r="B46" s="7"/>
       <c r="C46" s="7"/>
       <c r="D46" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -1779,7 +1844,7 @@
       <c r="B47" s="7"/>
       <c r="C47" s="7"/>
       <c r="D47" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -1788,7 +1853,7 @@
       <c r="B48" s="7"/>
       <c r="C48" s="7"/>
       <c r="D48" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -1797,7 +1862,7 @@
       <c r="B49" s="7"/>
       <c r="C49" s="7"/>
       <c r="D49" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -1806,7 +1871,7 @@
       <c r="B50" s="7"/>
       <c r="C50" s="7"/>
       <c r="D50" s="3" t="str">
-        <f t="shared" ref="D50:D51" si="1">IF(C50&lt;&gt;"",IF(B50&lt;&gt;"",B50-C50,"-"), "-")</f>
+        <f t="shared" ref="D50:D51" si="2">IF(C50&lt;&gt;"",IF(B50&lt;&gt;"",B50-C50,"-"), "-")</f>
         <v>-</v>
       </c>
     </row>
@@ -1815,7 +1880,7 @@
       <c r="B51" s="7"/>
       <c r="C51" s="7"/>
       <c r="D51" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Marble Madness - level 2 done, only 9 frames haead, a lot more lag in level transitions, emulation differences
</commit_message>
<xml_diff>
--- a/GenesisMarbleMadness/FrameCompare.xlsx
+++ b/GenesisMarbleMadness/FrameCompare.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\GenesisMarbleMadness\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08E1E183-C614-4AB1-9ADB-7189D0B5F51C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40C4DB42-36D4-467E-9F75-634D157335C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17670" yWindow="7965" windowWidth="10905" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="V5" sheetId="5" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="180">
   <si>
     <t>Place</t>
   </si>
@@ -564,7 +564,16 @@
     <t>Fadeout</t>
   </si>
   <si>
-    <t>Lv 2 Appears</t>
+    <t>Exit pipe</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>drawbridge down</t>
+  </si>
+  <si>
+    <t>Level 3 Title</t>
   </si>
 </sst>
 </file>
@@ -574,12 +583,19 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]&quot;-&quot;[$$-409]#,##0.00"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -913,118 +929,119 @@
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="6" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="6" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1348,11 +1365,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39B3565E-C480-4A10-8524-B7BC06C9B703}">
-  <dimension ref="A1:E190"/>
+  <dimension ref="A1:F201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1363,7 +1380,7 @@
     <col min="4" max="4" width="6.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1377,8 +1394,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="42" t="s">
+    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" s="34" t="s">
         <v>168</v>
       </c>
       <c r="B2" s="2">
@@ -1391,9 +1408,12 @@
         <f>IF(C2&lt;&gt;"",IF(B2&lt;&gt;"",C2-B2,"-"), "-")</f>
         <v>-1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="42" t="s">
+      <c r="F2" s="2">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="34" t="s">
         <v>169</v>
       </c>
       <c r="B3" s="2">
@@ -1406,27 +1426,33 @@
         <f>IF(C3&lt;&gt;"",IF(B3&lt;&gt;"",C3-B3,"-"), "-")</f>
         <v>-3</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="42" t="s">
+      <c r="F3" s="2">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="34" t="s">
         <v>170</v>
       </c>
       <c r="B4" s="2">
-        <v>405</v>
+        <v>427</v>
       </c>
       <c r="C4" s="2">
         <v>422</v>
       </c>
       <c r="D4" s="3">
-        <f t="shared" ref="D4:D16" si="0">IF(C4&lt;&gt;"",IF(B4&lt;&gt;"",C4-B4,"-"), "-")</f>
-        <v>17</v>
+        <f t="shared" ref="D4:D27" si="0">IF(C4&lt;&gt;"",IF(B4&lt;&gt;"",C4-B4,"-"), "-")</f>
+        <v>-5</v>
       </c>
       <c r="E4" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="42" t="s">
+      <c r="F4" s="2">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="34" t="s">
         <v>172</v>
       </c>
       <c r="B5" s="2">
@@ -1439,9 +1465,12 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="42" t="s">
+      <c r="F5" s="2">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6" s="34" t="s">
         <v>173</v>
       </c>
       <c r="B6" s="2">
@@ -1454,9 +1483,12 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="42" t="s">
+      <c r="F6" s="2">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A7" s="34" t="s">
         <v>174</v>
       </c>
       <c r="B7" s="2">
@@ -1469,9 +1501,12 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="42" t="s">
+      <c r="F7" s="2">
+        <v>1101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8" s="34" t="s">
         <v>175</v>
       </c>
       <c r="B8" s="2">
@@ -1484,160 +1519,192 @@
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="42" t="s">
-        <v>176</v>
-      </c>
-      <c r="B9" s="2"/>
+      <c r="F8" s="2">
+        <v>1316</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A9" s="43" t="s">
+        <v>152</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1433</v>
+      </c>
       <c r="C9" s="2">
         <v>1462</v>
       </c>
-      <c r="D9" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="42"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="33"/>
+      <c r="D9" s="3">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="F9" s="2">
+        <v>1438</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" s="43" t="s">
+        <v>168</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1455</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1484</v>
+      </c>
+      <c r="D10" s="3">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A11" s="43"/>
       <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="42" t="s">
-        <v>167</v>
+      <c r="C11" s="2">
+        <v>1665</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A12" s="43" t="s">
+        <v>173</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2">
+        <v>1671</v>
+      </c>
+      <c r="D12" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="F12" s="2">
+        <v>1646</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A13" s="43" t="s">
+        <v>177</v>
+      </c>
+      <c r="B13" s="2">
+        <v>1782</v>
+      </c>
+      <c r="C13" s="2">
+        <v>1806</v>
+      </c>
+      <c r="D13" s="3">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="F13" s="2">
+        <v>1801</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A14" s="43" t="s">
+        <v>178</v>
+      </c>
+      <c r="B14" s="2">
+        <v>1980</v>
+      </c>
+      <c r="C14" s="2">
+        <v>1996</v>
+      </c>
+      <c r="D14" s="3">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" s="43" t="s">
+        <v>176</v>
+      </c>
+      <c r="B15" s="2">
+        <v>2128</v>
+      </c>
+      <c r="C15" s="2">
+        <v>2137</v>
+      </c>
+      <c r="D15" s="3">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" s="43" t="s">
+        <v>179</v>
+      </c>
+      <c r="B16" s="2">
+        <v>2816</v>
+      </c>
+      <c r="C16" s="2">
+        <v>2825</v>
+      </c>
+      <c r="D16" s="3">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A17" s="43"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18" s="43"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" s="43"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A20" s="43"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="3"/>
+    </row>
+    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="43"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="3"/>
+    </row>
+    <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A22" s="33"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="3"/>
+    </row>
+    <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" s="34" t="s">
+        <v>167</v>
+      </c>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2">
         <v>7928</v>
       </c>
-      <c r="D12" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="D23" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7">
+      <c r="B24" s="7"/>
+      <c r="C24" s="7">
         <v>9567</v>
       </c>
-      <c r="D13" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="3" t="str">
-        <f>IF(C17&lt;&gt;"",IF(B17&lt;&gt;"",C17-B17,"-"), "-")</f>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="3" t="str">
-        <f>IF(C18&lt;&gt;"",IF(B18&lt;&gt;"",C18-B18,"-"), "-")</f>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="3" t="str">
-        <f>IF(C19&lt;&gt;"",IF(B19&lt;&gt;"",C19-B19,"-"), "-")</f>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="3" t="str">
-        <f>IF(C20&lt;&gt;"",IF(B20&lt;&gt;"",C20-B20,"-"), "-")</f>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="3" t="str">
-        <f>IF(C21&lt;&gt;"",IF(B21&lt;&gt;"",C21-B21,"-"), "-")</f>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="3" t="str">
-        <f>IF(C22&lt;&gt;"",IF(B22&lt;&gt;"",C22-B22,"-"), "-")</f>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="7"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="3" t="str">
-        <f>IF(C23&lt;&gt;"",IF(B23&lt;&gt;"",C23-B23,"-"), "-")</f>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
       <c r="D24" s="3" t="str">
-        <f>IF(C24&lt;&gt;"",IF(B24&lt;&gt;"",C24-B24,"-"), "-")</f>
+        <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
@@ -1646,7 +1713,7 @@
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
       <c r="D25" s="3" t="str">
-        <f>IF(C25&lt;&gt;"",IF(B25&lt;&gt;"",C25-B25,"-"), "-")</f>
+        <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
@@ -1655,7 +1722,7 @@
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
       <c r="D26" s="3" t="str">
-        <f>IF(C26&lt;&gt;"",IF(B26&lt;&gt;"",C26-B26,"-"), "-")</f>
+        <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
@@ -1664,7 +1731,7 @@
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
       <c r="D27" s="3" t="str">
-        <f>IF(C27&lt;&gt;"",IF(B27&lt;&gt;"",C27-B27,"-"), "-")</f>
+        <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
@@ -1673,7 +1740,7 @@
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
       <c r="D28" s="3" t="str">
-        <f>IF(C28&lt;&gt;"",IF(B28&lt;&gt;"",C28-B28,"-"), "-")</f>
+        <f t="shared" ref="D28:D55" si="1">IF(C28&lt;&gt;"",IF(B28&lt;&gt;"",C28-B28,"-"), "-")</f>
         <v>-</v>
       </c>
     </row>
@@ -1682,7 +1749,7 @@
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
       <c r="D29" s="3" t="str">
-        <f>IF(C29&lt;&gt;"",IF(B29&lt;&gt;"",C29-B29,"-"), "-")</f>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -1691,7 +1758,7 @@
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
       <c r="D30" s="3" t="str">
-        <f>IF(C30&lt;&gt;"",IF(B30&lt;&gt;"",C30-B30,"-"), "-")</f>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -1700,7 +1767,7 @@
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
       <c r="D31" s="3" t="str">
-        <f>IF(C31&lt;&gt;"",IF(B31&lt;&gt;"",C31-B31,"-"), "-")</f>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -1709,7 +1776,7 @@
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
       <c r="D32" s="3" t="str">
-        <f>IF(C32&lt;&gt;"",IF(B32&lt;&gt;"",C32-B32,"-"), "-")</f>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -1718,7 +1785,7 @@
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
       <c r="D33" s="3" t="str">
-        <f>IF(C33&lt;&gt;"",IF(B33&lt;&gt;"",C33-B33,"-"), "-")</f>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -1727,7 +1794,7 @@
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
       <c r="D34" s="3" t="str">
-        <f>IF(C34&lt;&gt;"",IF(B34&lt;&gt;"",C34-B34,"-"), "-")</f>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -1736,7 +1803,7 @@
       <c r="B35" s="7"/>
       <c r="C35" s="7"/>
       <c r="D35" s="3" t="str">
-        <f>IF(C35&lt;&gt;"",IF(B35&lt;&gt;"",C35-B35,"-"), "-")</f>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -1745,7 +1812,7 @@
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
       <c r="D36" s="3" t="str">
-        <f>IF(C36&lt;&gt;"",IF(B36&lt;&gt;"",C36-B36,"-"), "-")</f>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -1754,7 +1821,7 @@
       <c r="B37" s="7"/>
       <c r="C37" s="7"/>
       <c r="D37" s="3" t="str">
-        <f>IF(C37&lt;&gt;"",IF(B37&lt;&gt;"",C37-B37,"-"), "-")</f>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -1763,7 +1830,7 @@
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
       <c r="D38" s="3" t="str">
-        <f>IF(C38&lt;&gt;"",IF(B38&lt;&gt;"",C38-B38,"-"), "-")</f>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -1772,7 +1839,7 @@
       <c r="B39" s="7"/>
       <c r="C39" s="7"/>
       <c r="D39" s="3" t="str">
-        <f>IF(C39&lt;&gt;"",IF(B39&lt;&gt;"",C39-B39,"-"), "-")</f>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -1781,7 +1848,7 @@
       <c r="B40" s="7"/>
       <c r="C40" s="7"/>
       <c r="D40" s="3" t="str">
-        <f>IF(C40&lt;&gt;"",IF(B40&lt;&gt;"",C40-B40,"-"), "-")</f>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -1790,7 +1857,7 @@
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
       <c r="D41" s="3" t="str">
-        <f>IF(C41&lt;&gt;"",IF(B41&lt;&gt;"",C41-B41,"-"), "-")</f>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -1799,7 +1866,7 @@
       <c r="B42" s="7"/>
       <c r="C42" s="7"/>
       <c r="D42" s="3" t="str">
-        <f>IF(C42&lt;&gt;"",IF(B42&lt;&gt;"",C42-B42,"-"), "-")</f>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -1808,7 +1875,7 @@
       <c r="B43" s="7"/>
       <c r="C43" s="7"/>
       <c r="D43" s="3" t="str">
-        <f>IF(C43&lt;&gt;"",IF(B43&lt;&gt;"",C43-B43,"-"), "-")</f>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -1817,7 +1884,7 @@
       <c r="B44" s="7"/>
       <c r="C44" s="7"/>
       <c r="D44" s="3" t="str">
-        <f>IF(C44&lt;&gt;"",IF(B44&lt;&gt;"",C44-B44,"-"), "-")</f>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -1826,7 +1893,7 @@
       <c r="B45" s="7"/>
       <c r="C45" s="7"/>
       <c r="D45" s="3" t="str">
-        <f t="shared" ref="D45:D49" si="1">IF(C45&lt;&gt;"",IF(B45&lt;&gt;"",C45-B45,"-"), "-")</f>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -1871,7 +1938,7 @@
       <c r="B50" s="7"/>
       <c r="C50" s="7"/>
       <c r="D50" s="3" t="str">
-        <f t="shared" ref="D50:D51" si="2">IF(C50&lt;&gt;"",IF(B50&lt;&gt;"",B50-C50,"-"), "-")</f>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -1880,7 +1947,7 @@
       <c r="B51" s="7"/>
       <c r="C51" s="7"/>
       <c r="D51" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -1888,53 +1955,108 @@
       <c r="A52" s="7"/>
       <c r="B52" s="7"/>
       <c r="C52" s="7"/>
+      <c r="D52" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="53" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="7"/>
       <c r="B53" s="7"/>
       <c r="C53" s="7"/>
+      <c r="D53" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="54" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A54" s="7"/>
       <c r="B54" s="7"/>
       <c r="C54" s="7"/>
+      <c r="D54" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="55" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A55" s="7"/>
       <c r="B55" s="7"/>
       <c r="C55" s="7"/>
+      <c r="D55" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="56" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A56" s="7"/>
       <c r="B56" s="7"/>
       <c r="C56" s="7"/>
+      <c r="D56" s="3" t="str">
+        <f t="shared" ref="D56:D60" si="2">IF(C56&lt;&gt;"",IF(B56&lt;&gt;"",C56-B56,"-"), "-")</f>
+        <v>-</v>
+      </c>
     </row>
     <row r="57" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A57" s="7"/>
       <c r="B57" s="7"/>
       <c r="C57" s="7"/>
+      <c r="D57" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="58" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A58" s="7"/>
       <c r="B58" s="7"/>
       <c r="C58" s="7"/>
+      <c r="D58" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="59" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A59" s="7"/>
       <c r="B59" s="7"/>
       <c r="C59" s="7"/>
+      <c r="D59" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="60" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A60" s="7"/>
       <c r="B60" s="7"/>
       <c r="C60" s="7"/>
+      <c r="D60" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="61" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A61" s="7"/>
       <c r="B61" s="7"/>
       <c r="C61" s="7"/>
+      <c r="D61" s="3" t="str">
+        <f t="shared" ref="D61:D62" si="3">IF(C61&lt;&gt;"",IF(B61&lt;&gt;"",B61-C61,"-"), "-")</f>
+        <v>-</v>
+      </c>
     </row>
     <row r="62" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A62" s="7"/>
       <c r="B62" s="7"/>
       <c r="C62" s="7"/>
+      <c r="D62" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="63" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A63" s="7"/>
       <c r="B63" s="7"/>
       <c r="C63" s="7"/>
     </row>
     <row r="64" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A64" s="7"/>
       <c r="B64" s="7"/>
       <c r="C64" s="7"/>
     </row>
@@ -2441,6 +2563,50 @@
     <row r="190" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B190" s="7"/>
       <c r="C190" s="7"/>
+    </row>
+    <row r="191" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B191" s="7"/>
+      <c r="C191" s="7"/>
+    </row>
+    <row r="192" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B192" s="7"/>
+      <c r="C192" s="7"/>
+    </row>
+    <row r="193" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B193" s="7"/>
+      <c r="C193" s="7"/>
+    </row>
+    <row r="194" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B194" s="7"/>
+      <c r="C194" s="7"/>
+    </row>
+    <row r="195" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B195" s="7"/>
+      <c r="C195" s="7"/>
+    </row>
+    <row r="196" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B196" s="7"/>
+      <c r="C196" s="7"/>
+    </row>
+    <row r="197" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B197" s="7"/>
+      <c r="C197" s="7"/>
+    </row>
+    <row r="198" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B198" s="7"/>
+      <c r="C198" s="7"/>
+    </row>
+    <row r="199" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B199" s="7"/>
+      <c r="C199" s="7"/>
+    </row>
+    <row r="200" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B200" s="7"/>
+      <c r="C200" s="7"/>
+    </row>
+    <row r="201" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B201" s="7"/>
+      <c r="C201" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8493,7 +8659,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="15" type="noConversion"/>
+  <phoneticPr fontId="16" type="noConversion"/>
   <pageMargins left="0" right="0" top="0.39410000000000006" bottom="0.39410000000000006" header="0" footer="0"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <headerFooter>
@@ -8528,10 +8694,10 @@
       <c r="H1" s="14"/>
       <c r="I1" s="14"/>
       <c r="J1" s="15"/>
-      <c r="K1" s="34" t="s">
+      <c r="K1" s="35" t="s">
         <v>157</v>
       </c>
-      <c r="L1" s="35"/>
+      <c r="L1" s="36"/>
     </row>
     <row r="2" spans="1:12" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
@@ -10383,13 +10549,13 @@
       <c r="G53" s="17" t="s">
         <v>157</v>
       </c>
-      <c r="H53" s="36" t="s">
+      <c r="H53" s="37" t="s">
         <v>164</v>
       </c>
-      <c r="I53" s="37"/>
-      <c r="J53" s="37"/>
-      <c r="K53" s="37"/>
-      <c r="L53" s="38"/>
+      <c r="I53" s="38"/>
+      <c r="J53" s="38"/>
+      <c r="K53" s="38"/>
+      <c r="L53" s="39"/>
     </row>
     <row r="54" spans="1:12" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A54" s="11"/>
@@ -10411,11 +10577,11 @@
       <c r="G54" s="27">
         <v>31536</v>
       </c>
-      <c r="H54" s="39"/>
-      <c r="I54" s="40"/>
-      <c r="J54" s="40"/>
-      <c r="K54" s="40"/>
-      <c r="L54" s="41"/>
+      <c r="H54" s="40"/>
+      <c r="I54" s="41"/>
+      <c r="J54" s="41"/>
+      <c r="K54" s="41"/>
+      <c r="L54" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
marble madness - cleanup and start v3
</commit_message>
<xml_diff>
--- a/GenesisMarbleMadness/FrameCompare.xlsx
+++ b/GenesisMarbleMadness/FrameCompare.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\GenesisMarbleMadness\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D30B01BF-1CF0-4A65-91FE-1FB99958E9D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BC76793-B92A-4333-8459-D59248B9B536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-12375" yWindow="1650" windowWidth="10905" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="V2" sheetId="5" r:id="rId1"/>
+    <sheet name="V3" sheetId="7" r:id="rId1"/>
+    <sheet name="V2" sheetId="5" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="32">
   <si>
     <t>Place</t>
   </si>
@@ -120,6 +121,12 @@
   </si>
   <si>
     <t>3rd platform move</t>
+  </si>
+  <si>
+    <t>V3</t>
+  </si>
+  <si>
+    <t>Note: One Player, Pick Hard, Standard</t>
   </si>
 </sst>
 </file>
@@ -597,10 +604,1336 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A88CD45-A2B6-49C4-A4B2-BB74C4A0A2BD}">
+  <dimension ref="A1:F208"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.25" customWidth="1"/>
+    <col min="2" max="3" width="8.75" customWidth="1"/>
+    <col min="4" max="4" width="6.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2">
+        <v>181</v>
+      </c>
+      <c r="D2" s="3" t="str">
+        <f>IF(C2&lt;&gt;"",IF(B2&lt;&gt;"",C2-B2,"-"), "-")</f>
+        <v>-</v>
+      </c>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2">
+        <v>294</v>
+      </c>
+      <c r="D3" s="3" t="str">
+        <f>IF(C3&lt;&gt;"",IF(B3&lt;&gt;"",C3-B3,"-"), "-")</f>
+        <v>-</v>
+      </c>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2">
+        <v>427</v>
+      </c>
+      <c r="D4" s="3" t="str">
+        <f t="shared" ref="D4:D67" si="0">IF(C4&lt;&gt;"",IF(B4&lt;&gt;"",C4-B4,"-"), "-")</f>
+        <v>-</v>
+      </c>
+      <c r="E4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="10">
+        <v>526</v>
+      </c>
+      <c r="C5" s="2">
+        <v>569</v>
+      </c>
+      <c r="D5" s="3">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2">
+        <v>736</v>
+      </c>
+      <c r="D6" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2">
+        <v>1101</v>
+      </c>
+      <c r="D7" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2">
+        <v>1316</v>
+      </c>
+      <c r="D8" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2">
+        <v>1433</v>
+      </c>
+      <c r="D9" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2">
+        <v>1455</v>
+      </c>
+      <c r="D10" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="3"/>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2">
+        <v>1782</v>
+      </c>
+      <c r="D13" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2">
+        <v>1980</v>
+      </c>
+      <c r="D14" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2">
+        <v>2128</v>
+      </c>
+      <c r="D15" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2">
+        <v>2816</v>
+      </c>
+      <c r="D16" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2">
+        <v>3449</v>
+      </c>
+      <c r="D17" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2">
+        <v>3894</v>
+      </c>
+      <c r="D18" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2">
+        <v>4014</v>
+      </c>
+      <c r="D19" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2">
+        <v>4939</v>
+      </c>
+      <c r="D20" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2">
+        <v>5218</v>
+      </c>
+      <c r="D21" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2">
+        <v>5394</v>
+      </c>
+      <c r="D22" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2">
+        <v>5540</v>
+      </c>
+      <c r="D23" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2">
+        <v>5851</v>
+      </c>
+      <c r="D24" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" s="8"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="3"/>
+    </row>
+    <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2">
+        <v>6894</v>
+      </c>
+      <c r="D26" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2">
+        <v>7722</v>
+      </c>
+      <c r="D27" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A28" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2">
+        <v>7822</v>
+      </c>
+      <c r="D28" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A29" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2">
+        <v>7918</v>
+      </c>
+      <c r="D29" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2">
+        <v>7924</v>
+      </c>
+      <c r="D30" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A32" s="5"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A33" s="5"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A34" s="5"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A35" s="5"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A36" s="5"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A37" s="5"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A38" s="5"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A39" s="5"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A40" s="5"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A41" s="5"/>
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A42" s="5"/>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A43" s="5"/>
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A44" s="5"/>
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A45" s="5"/>
+      <c r="B45" s="5"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A46" s="5"/>
+      <c r="B46" s="5"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A47" s="5"/>
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A48" s="5"/>
+      <c r="B48" s="5"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A49" s="5"/>
+      <c r="B49" s="5"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A50" s="5"/>
+      <c r="B50" s="5"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A51" s="5"/>
+      <c r="B51" s="5"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A52" s="5"/>
+      <c r="B52" s="5"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A53" s="5"/>
+      <c r="B53" s="5"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A54" s="5"/>
+      <c r="B54" s="5"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A55" s="5"/>
+      <c r="B55" s="5"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A56" s="5"/>
+      <c r="B56" s="5"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A57" s="5"/>
+      <c r="B57" s="5"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A58" s="5"/>
+      <c r="B58" s="5"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A59" s="5"/>
+      <c r="B59" s="5"/>
+      <c r="C59" s="5"/>
+      <c r="D59" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A60" s="5"/>
+      <c r="B60" s="5"/>
+      <c r="C60" s="5"/>
+      <c r="D60" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A61" s="5"/>
+      <c r="B61" s="5"/>
+      <c r="C61" s="5"/>
+      <c r="D61" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A62" s="5"/>
+      <c r="B62" s="5"/>
+      <c r="C62" s="5"/>
+      <c r="D62" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A63" s="5"/>
+      <c r="B63" s="5"/>
+      <c r="C63" s="5"/>
+      <c r="D63" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A64" s="5"/>
+      <c r="B64" s="5"/>
+      <c r="C64" s="5"/>
+      <c r="D64" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A65" s="5"/>
+      <c r="B65" s="5"/>
+      <c r="C65" s="5"/>
+      <c r="D65" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A66" s="5"/>
+      <c r="B66" s="5"/>
+      <c r="C66" s="5"/>
+      <c r="D66" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A67" s="5"/>
+      <c r="B67" s="5"/>
+      <c r="C67" s="5"/>
+      <c r="D67" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A68" s="5"/>
+      <c r="B68" s="5"/>
+      <c r="C68" s="5"/>
+      <c r="D68" s="3" t="str">
+        <f t="shared" ref="D68:D69" si="1">IF(C68&lt;&gt;"",IF(B68&lt;&gt;"",B68-C68,"-"), "-")</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A69" s="5"/>
+      <c r="B69" s="5"/>
+      <c r="C69" s="5"/>
+      <c r="D69" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A70" s="5"/>
+      <c r="B70" s="5"/>
+      <c r="C70" s="5"/>
+    </row>
+    <row r="71" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A71" s="5"/>
+      <c r="B71" s="5"/>
+      <c r="C71" s="5"/>
+    </row>
+    <row r="72" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B72" s="5"/>
+      <c r="C72" s="5"/>
+    </row>
+    <row r="73" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B73" s="5"/>
+      <c r="C73" s="5"/>
+    </row>
+    <row r="74" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B74" s="5"/>
+      <c r="C74" s="5"/>
+    </row>
+    <row r="75" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B75" s="5"/>
+      <c r="C75" s="5"/>
+    </row>
+    <row r="76" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B76" s="5"/>
+      <c r="C76" s="5"/>
+    </row>
+    <row r="77" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B77" s="5"/>
+      <c r="C77" s="5"/>
+    </row>
+    <row r="78" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B78" s="5"/>
+      <c r="C78" s="5"/>
+    </row>
+    <row r="79" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B79" s="5"/>
+      <c r="C79" s="5"/>
+    </row>
+    <row r="80" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B80" s="5"/>
+      <c r="C80" s="5"/>
+    </row>
+    <row r="81" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B81" s="5"/>
+      <c r="C81" s="5"/>
+    </row>
+    <row r="82" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B82" s="5"/>
+      <c r="C82" s="5"/>
+    </row>
+    <row r="83" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B83" s="5"/>
+      <c r="C83" s="5"/>
+    </row>
+    <row r="84" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B84" s="5"/>
+      <c r="C84" s="5"/>
+    </row>
+    <row r="85" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B85" s="5"/>
+      <c r="C85" s="5"/>
+    </row>
+    <row r="86" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B86" s="5"/>
+      <c r="C86" s="5"/>
+    </row>
+    <row r="87" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B87" s="5"/>
+      <c r="C87" s="5"/>
+    </row>
+    <row r="88" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B88" s="5"/>
+      <c r="C88" s="5"/>
+    </row>
+    <row r="89" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B89" s="5"/>
+      <c r="C89" s="5"/>
+    </row>
+    <row r="90" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B90" s="5"/>
+      <c r="C90" s="5"/>
+    </row>
+    <row r="91" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B91" s="5"/>
+      <c r="C91" s="5"/>
+    </row>
+    <row r="92" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B92" s="5"/>
+      <c r="C92" s="5"/>
+    </row>
+    <row r="93" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B93" s="5"/>
+      <c r="C93" s="5"/>
+    </row>
+    <row r="94" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B94" s="5"/>
+      <c r="C94" s="5"/>
+    </row>
+    <row r="95" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B95" s="5"/>
+      <c r="C95" s="5"/>
+    </row>
+    <row r="96" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B96" s="5"/>
+      <c r="C96" s="5"/>
+    </row>
+    <row r="97" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B97" s="5"/>
+      <c r="C97" s="5"/>
+    </row>
+    <row r="98" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B98" s="5"/>
+      <c r="C98" s="5"/>
+    </row>
+    <row r="99" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B99" s="5"/>
+      <c r="C99" s="5"/>
+    </row>
+    <row r="100" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B100" s="5"/>
+      <c r="C100" s="5"/>
+    </row>
+    <row r="101" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B101" s="5"/>
+      <c r="C101" s="5"/>
+    </row>
+    <row r="102" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B102" s="5"/>
+      <c r="C102" s="5"/>
+    </row>
+    <row r="103" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B103" s="5"/>
+      <c r="C103" s="5"/>
+    </row>
+    <row r="104" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B104" s="5"/>
+      <c r="C104" s="5"/>
+    </row>
+    <row r="105" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B105" s="5"/>
+      <c r="C105" s="5"/>
+    </row>
+    <row r="106" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B106" s="5"/>
+      <c r="C106" s="5"/>
+    </row>
+    <row r="107" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B107" s="5"/>
+      <c r="C107" s="5"/>
+    </row>
+    <row r="108" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B108" s="5"/>
+      <c r="C108" s="5"/>
+    </row>
+    <row r="109" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B109" s="5"/>
+      <c r="C109" s="5"/>
+    </row>
+    <row r="110" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B110" s="5"/>
+      <c r="C110" s="5"/>
+    </row>
+    <row r="111" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B111" s="5"/>
+      <c r="C111" s="5"/>
+    </row>
+    <row r="112" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B112" s="5"/>
+      <c r="C112" s="5"/>
+    </row>
+    <row r="113" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B113" s="5"/>
+      <c r="C113" s="5"/>
+    </row>
+    <row r="114" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B114" s="5"/>
+      <c r="C114" s="5"/>
+    </row>
+    <row r="115" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B115" s="5"/>
+      <c r="C115" s="5"/>
+    </row>
+    <row r="116" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B116" s="5"/>
+      <c r="C116" s="5"/>
+    </row>
+    <row r="117" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B117" s="5"/>
+      <c r="C117" s="5"/>
+    </row>
+    <row r="118" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B118" s="5"/>
+      <c r="C118" s="5"/>
+    </row>
+    <row r="119" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B119" s="5"/>
+      <c r="C119" s="5"/>
+    </row>
+    <row r="120" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B120" s="5"/>
+      <c r="C120" s="5"/>
+    </row>
+    <row r="121" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B121" s="5"/>
+      <c r="C121" s="5"/>
+    </row>
+    <row r="122" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B122" s="5"/>
+      <c r="C122" s="5"/>
+    </row>
+    <row r="123" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B123" s="5"/>
+      <c r="C123" s="5"/>
+    </row>
+    <row r="124" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B124" s="5"/>
+      <c r="C124" s="5"/>
+    </row>
+    <row r="125" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B125" s="5"/>
+      <c r="C125" s="5"/>
+    </row>
+    <row r="126" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B126" s="5"/>
+      <c r="C126" s="5"/>
+    </row>
+    <row r="127" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B127" s="5"/>
+      <c r="C127" s="5"/>
+    </row>
+    <row r="128" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B128" s="5"/>
+      <c r="C128" s="5"/>
+    </row>
+    <row r="129" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B129" s="5"/>
+      <c r="C129" s="5"/>
+    </row>
+    <row r="130" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B130" s="5"/>
+      <c r="C130" s="5"/>
+    </row>
+    <row r="131" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B131" s="5"/>
+      <c r="C131" s="5"/>
+    </row>
+    <row r="132" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B132" s="5"/>
+      <c r="C132" s="5"/>
+    </row>
+    <row r="133" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B133" s="5"/>
+      <c r="C133" s="5"/>
+    </row>
+    <row r="134" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B134" s="5"/>
+      <c r="C134" s="5"/>
+    </row>
+    <row r="135" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B135" s="5"/>
+      <c r="C135" s="5"/>
+    </row>
+    <row r="136" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B136" s="5"/>
+      <c r="C136" s="5"/>
+    </row>
+    <row r="137" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B137" s="5"/>
+      <c r="C137" s="5"/>
+    </row>
+    <row r="138" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B138" s="5"/>
+      <c r="C138" s="5"/>
+    </row>
+    <row r="139" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B139" s="5"/>
+      <c r="C139" s="5"/>
+    </row>
+    <row r="140" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B140" s="5"/>
+      <c r="C140" s="5"/>
+    </row>
+    <row r="141" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B141" s="5"/>
+      <c r="C141" s="5"/>
+    </row>
+    <row r="142" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B142" s="5"/>
+      <c r="C142" s="5"/>
+    </row>
+    <row r="143" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B143" s="5"/>
+      <c r="C143" s="5"/>
+    </row>
+    <row r="144" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B144" s="5"/>
+      <c r="C144" s="5"/>
+    </row>
+    <row r="145" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B145" s="5"/>
+      <c r="C145" s="5"/>
+    </row>
+    <row r="146" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B146" s="5"/>
+      <c r="C146" s="5"/>
+    </row>
+    <row r="147" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B147" s="5"/>
+      <c r="C147" s="5"/>
+    </row>
+    <row r="148" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B148" s="5"/>
+      <c r="C148" s="5"/>
+    </row>
+    <row r="149" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B149" s="5"/>
+      <c r="C149" s="5"/>
+    </row>
+    <row r="150" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B150" s="5"/>
+      <c r="C150" s="5"/>
+    </row>
+    <row r="151" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B151" s="5"/>
+      <c r="C151" s="5"/>
+    </row>
+    <row r="152" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B152" s="5"/>
+      <c r="C152" s="5"/>
+    </row>
+    <row r="153" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B153" s="5"/>
+      <c r="C153" s="5"/>
+    </row>
+    <row r="154" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B154" s="5"/>
+      <c r="C154" s="5"/>
+    </row>
+    <row r="155" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B155" s="5"/>
+      <c r="C155" s="5"/>
+    </row>
+    <row r="156" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B156" s="5"/>
+      <c r="C156" s="5"/>
+    </row>
+    <row r="157" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B157" s="5"/>
+      <c r="C157" s="5"/>
+    </row>
+    <row r="158" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B158" s="5"/>
+      <c r="C158" s="5"/>
+    </row>
+    <row r="159" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B159" s="5"/>
+      <c r="C159" s="5"/>
+    </row>
+    <row r="160" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B160" s="5"/>
+      <c r="C160" s="5"/>
+    </row>
+    <row r="161" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B161" s="5"/>
+      <c r="C161" s="5"/>
+    </row>
+    <row r="162" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B162" s="5"/>
+      <c r="C162" s="5"/>
+    </row>
+    <row r="163" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B163" s="5"/>
+      <c r="C163" s="5"/>
+    </row>
+    <row r="164" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B164" s="5"/>
+      <c r="C164" s="5"/>
+    </row>
+    <row r="165" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B165" s="5"/>
+      <c r="C165" s="5"/>
+    </row>
+    <row r="166" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B166" s="5"/>
+      <c r="C166" s="5"/>
+    </row>
+    <row r="167" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B167" s="5"/>
+      <c r="C167" s="5"/>
+    </row>
+    <row r="168" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B168" s="5"/>
+      <c r="C168" s="5"/>
+    </row>
+    <row r="169" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B169" s="5"/>
+      <c r="C169" s="5"/>
+    </row>
+    <row r="170" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B170" s="5"/>
+      <c r="C170" s="5"/>
+    </row>
+    <row r="171" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B171" s="5"/>
+      <c r="C171" s="5"/>
+    </row>
+    <row r="172" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B172" s="5"/>
+      <c r="C172" s="5"/>
+    </row>
+    <row r="173" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B173" s="5"/>
+      <c r="C173" s="5"/>
+    </row>
+    <row r="174" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B174" s="5"/>
+      <c r="C174" s="5"/>
+    </row>
+    <row r="175" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B175" s="5"/>
+      <c r="C175" s="5"/>
+    </row>
+    <row r="176" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B176" s="5"/>
+      <c r="C176" s="5"/>
+    </row>
+    <row r="177" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B177" s="5"/>
+      <c r="C177" s="5"/>
+    </row>
+    <row r="178" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B178" s="5"/>
+      <c r="C178" s="5"/>
+    </row>
+    <row r="179" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B179" s="5"/>
+      <c r="C179" s="5"/>
+    </row>
+    <row r="180" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B180" s="5"/>
+      <c r="C180" s="5"/>
+    </row>
+    <row r="181" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B181" s="5"/>
+      <c r="C181" s="5"/>
+    </row>
+    <row r="182" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B182" s="5"/>
+      <c r="C182" s="5"/>
+    </row>
+    <row r="183" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B183" s="5"/>
+      <c r="C183" s="5"/>
+    </row>
+    <row r="184" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B184" s="5"/>
+      <c r="C184" s="5"/>
+    </row>
+    <row r="185" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B185" s="5"/>
+      <c r="C185" s="5"/>
+    </row>
+    <row r="186" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B186" s="5"/>
+      <c r="C186" s="5"/>
+    </row>
+    <row r="187" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B187" s="5"/>
+      <c r="C187" s="5"/>
+    </row>
+    <row r="188" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B188" s="5"/>
+      <c r="C188" s="5"/>
+    </row>
+    <row r="189" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B189" s="5"/>
+      <c r="C189" s="5"/>
+    </row>
+    <row r="190" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B190" s="5"/>
+      <c r="C190" s="5"/>
+    </row>
+    <row r="191" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B191" s="5"/>
+      <c r="C191" s="5"/>
+    </row>
+    <row r="192" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B192" s="5"/>
+      <c r="C192" s="5"/>
+    </row>
+    <row r="193" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B193" s="5"/>
+      <c r="C193" s="5"/>
+    </row>
+    <row r="194" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B194" s="5"/>
+      <c r="C194" s="5"/>
+    </row>
+    <row r="195" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B195" s="5"/>
+      <c r="C195" s="5"/>
+    </row>
+    <row r="196" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B196" s="5"/>
+      <c r="C196" s="5"/>
+    </row>
+    <row r="197" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B197" s="5"/>
+      <c r="C197" s="5"/>
+    </row>
+    <row r="198" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B198" s="5"/>
+      <c r="C198" s="5"/>
+    </row>
+    <row r="199" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B199" s="5"/>
+      <c r="C199" s="5"/>
+    </row>
+    <row r="200" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B200" s="5"/>
+      <c r="C200" s="5"/>
+    </row>
+    <row r="201" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B201" s="5"/>
+      <c r="C201" s="5"/>
+    </row>
+    <row r="202" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B202" s="5"/>
+      <c r="C202" s="5"/>
+    </row>
+    <row r="203" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B203" s="5"/>
+      <c r="C203" s="5"/>
+    </row>
+    <row r="204" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B204" s="5"/>
+      <c r="C204" s="5"/>
+    </row>
+    <row r="205" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B205" s="5"/>
+      <c r="C205" s="5"/>
+    </row>
+    <row r="206" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B206" s="5"/>
+      <c r="C206" s="5"/>
+    </row>
+    <row r="207" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B207" s="5"/>
+      <c r="C207" s="5"/>
+    </row>
+    <row r="208" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B208" s="5"/>
+      <c r="C208" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39B3565E-C480-4A10-8524-B7BC06C9B703}">
   <dimension ref="A1:F208"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C30" sqref="C30"/>
     </sheetView>

</xml_diff>

<commit_message>
mm v3 - level 1 done 33 ahead
</commit_message>
<xml_diff>
--- a/GenesisMarbleMadness/FrameCompare.xlsx
+++ b/GenesisMarbleMadness/FrameCompare.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\GenesisMarbleMadness\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BC76793-B92A-4333-8459-D59248B9B536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E09C3F4-53E8-4B83-8F35-EDBBA1E3BD0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-12375" yWindow="1650" windowWidth="10905" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-7950" yWindow="300" windowWidth="7965" windowHeight="12825" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="V3" sheetId="7" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="45">
   <si>
     <t>Place</t>
   </si>
@@ -127,6 +127,45 @@
   </si>
   <si>
     <t>Note: One Player, Pick Hard, Standard</t>
+  </si>
+  <si>
+    <t>1st input frame</t>
+  </si>
+  <si>
+    <t>D = DR</t>
+  </si>
+  <si>
+    <t>DL = D</t>
+  </si>
+  <si>
+    <t>L = DL</t>
+  </si>
+  <si>
+    <t>LU = L</t>
+  </si>
+  <si>
+    <t>U = LU</t>
+  </si>
+  <si>
+    <t>UR = U</t>
+  </si>
+  <si>
+    <t>R = UR</t>
+  </si>
+  <si>
+    <t>RD = R</t>
+  </si>
+  <si>
+    <t>crash</t>
+  </si>
+  <si>
+    <t>Y = 178</t>
+  </si>
+  <si>
+    <t>leap crash</t>
+  </si>
+  <si>
+    <t>about to leap</t>
   </si>
 </sst>
 </file>
@@ -136,12 +175,26 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]&quot;-&quot;[$$-409]#,##0.00"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -262,22 +315,24 @@
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="6" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="6" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -605,11 +660,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A88CD45-A2B6-49C4-A4B2-BB74C4A0A2BD}">
-  <dimension ref="A1:F208"/>
+  <dimension ref="A1:F212"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
+      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -635,423 +690,475 @@
     </row>
     <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2">
-        <v>181</v>
+        <v>427</v>
       </c>
       <c r="D2" s="3" t="str">
-        <f>IF(C2&lt;&gt;"",IF(B2&lt;&gt;"",C2-B2,"-"), "-")</f>
+        <f t="shared" ref="D2:D71" si="0">IF(C2&lt;&gt;"",IF(B2&lt;&gt;"",C2-B2,"-"), "-")</f>
         <v>-</v>
       </c>
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="2"/>
+        <v>11</v>
+      </c>
+      <c r="B3" s="10">
+        <v>526</v>
+      </c>
       <c r="C3" s="2">
-        <v>294</v>
-      </c>
-      <c r="D3" s="3" t="str">
-        <f>IF(C3&lt;&gt;"",IF(B3&lt;&gt;"",C3-B3,"-"), "-")</f>
-        <v>-</v>
+        <v>569</v>
+      </c>
+      <c r="D3" s="3">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="E3" t="s">
+        <v>31</v>
       </c>
       <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="2"/>
+      <c r="A4" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="10">
+        <v>707</v>
+      </c>
       <c r="C4" s="2">
-        <v>427</v>
-      </c>
-      <c r="D4" s="3" t="str">
-        <f t="shared" ref="D4:D67" si="0">IF(C4&lt;&gt;"",IF(B4&lt;&gt;"",C4-B4,"-"), "-")</f>
-        <v>-</v>
-      </c>
-      <c r="E4" t="s">
-        <v>31</v>
+        <v>750</v>
+      </c>
+      <c r="D4" s="3">
+        <f t="shared" si="0"/>
+        <v>43</v>
       </c>
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>11</v>
+      <c r="A5" s="12" t="s">
+        <v>25</v>
       </c>
       <c r="B5" s="10">
-        <v>526</v>
+        <v>716</v>
       </c>
       <c r="C5" s="2">
-        <v>569</v>
+        <v>757</v>
       </c>
       <c r="D5" s="3">
         <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="10">
+        <v>727</v>
+      </c>
+      <c r="C6" s="2">
+        <v>764</v>
+      </c>
+      <c r="D6" s="3">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="10">
+        <v>860</v>
+      </c>
+      <c r="C7" s="2">
+        <v>899</v>
+      </c>
+      <c r="D7" s="3">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="10">
+        <v>950</v>
+      </c>
+      <c r="C8" s="2">
+        <v>989</v>
+      </c>
+      <c r="D8" s="3">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="10">
+        <v>992</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1029</v>
+      </c>
+      <c r="D9" s="3">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2">
-        <v>736</v>
-      </c>
-      <c r="D6" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="B10" s="2">
+        <v>1005</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1044</v>
+      </c>
+      <c r="D10" s="3">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2">
-        <v>1101</v>
-      </c>
-      <c r="D7" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2">
-        <v>1316</v>
-      </c>
-      <c r="D8" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2">
-        <v>1433</v>
-      </c>
-      <c r="D9" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2">
-        <v>1455</v>
-      </c>
-      <c r="D10" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="3"/>
-      <c r="F11" s="2"/>
+      <c r="B11" s="2">
+        <v>1060</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1093</v>
+      </c>
+      <c r="D11" s="3">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="E11">
+        <f>C11-41</f>
+        <v>1052</v>
+      </c>
+      <c r="F11" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F12" s="2"/>
+        <v>7</v>
+      </c>
+      <c r="B12" s="2">
+        <v>1422</v>
+      </c>
+      <c r="C12" s="2">
+        <v>1455</v>
+      </c>
+      <c r="D12" s="3">
+        <f t="shared" ref="D12" si="1">IF(C12&lt;&gt;"",IF(B12&lt;&gt;"",C12-B12,"-"), "-")</f>
+        <v>33</v>
+      </c>
+      <c r="F12" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B13" s="2"/>
-      <c r="C13" s="2">
-        <v>1782</v>
-      </c>
+      <c r="C13" s="2"/>
       <c r="D13" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="F13" s="2"/>
+      <c r="F13" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
-        <v>17</v>
-      </c>
+      <c r="A14" s="7"/>
       <c r="B14" s="2"/>
-      <c r="C14" s="2">
-        <v>1980</v>
-      </c>
+      <c r="C14" s="2"/>
       <c r="D14" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="F14" s="2"/>
+      <c r="F14" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
-        <v>15</v>
-      </c>
+      <c r="A15" s="7"/>
       <c r="B15" s="2"/>
-      <c r="C15" s="2">
-        <v>2128</v>
-      </c>
-      <c r="D15" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="C15" s="2"/>
+      <c r="D15" s="3"/>
+      <c r="F15" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B16" s="2"/>
-      <c r="C16" s="2">
-        <v>2816</v>
-      </c>
+      <c r="C16" s="2"/>
       <c r="D16" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="F16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2">
-        <v>3449</v>
+        <v>1782</v>
       </c>
       <c r="D17" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
-        <v>19</v>
+      <c r="F17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2">
-        <v>3894</v>
+        <v>1980</v>
       </c>
       <c r="D18" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
-        <v>20</v>
+      <c r="F18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>15</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2">
-        <v>4014</v>
+        <v>2128</v>
       </c>
       <c r="D19" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
-        <v>22</v>
+    <row r="20" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>18</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2">
-        <v>4939</v>
+        <v>2816</v>
       </c>
       <c r="D20" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
-        <v>21</v>
+    <row r="21" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>15</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2">
-        <v>5218</v>
+        <v>3449</v>
       </c>
       <c r="D21" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2">
-        <v>5394</v>
+        <v>3894</v>
       </c>
       <c r="D22" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2">
-        <v>5540</v>
+        <v>4014</v>
       </c>
       <c r="D23" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2">
-        <v>5851</v>
+        <v>4939</v>
       </c>
       <c r="D24" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
+    <row r="25" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>21</v>
+      </c>
       <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="3"/>
-    </row>
-    <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="9" t="s">
-        <v>26</v>
+      <c r="C25" s="2">
+        <v>5218</v>
+      </c>
+      <c r="D25" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
+        <v>23</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2">
-        <v>6894</v>
+        <v>5394</v>
       </c>
       <c r="D26" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A27" s="9" t="s">
-        <v>27</v>
+    <row r="27" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
+        <v>25</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2">
-        <v>7722</v>
+        <v>5540</v>
       </c>
       <c r="D27" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="10" t="s">
-        <v>28</v>
+    <row r="28" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
+        <v>24</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2">
-        <v>7822</v>
+        <v>5851</v>
       </c>
       <c r="D28" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A29" s="10" t="s">
-        <v>29</v>
-      </c>
+    <row r="29" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A29" s="8"/>
       <c r="B29" s="2"/>
-      <c r="C29" s="2">
-        <v>7918</v>
-      </c>
-      <c r="D29" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
-        <v>6</v>
+      <c r="C29" s="2"/>
+      <c r="D29" s="3"/>
+    </row>
+    <row r="30" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
+        <v>26</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="2">
+        <v>6894</v>
+      </c>
+      <c r="D30" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2">
+        <v>7722</v>
+      </c>
+      <c r="D31" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A32" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2">
+        <v>7822</v>
+      </c>
+      <c r="D32" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A33" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2">
+        <v>7918</v>
+      </c>
+      <c r="D33" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2">
         <v>7924</v>
       </c>
-      <c r="D30" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
+      <c r="D34" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A32" s="5"/>
-      <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A33" s="5"/>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A34" s="5"/>
-      <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A35" s="5"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="3" t="str">
@@ -1352,7 +1459,7 @@
       <c r="B68" s="5"/>
       <c r="C68" s="5"/>
       <c r="D68" s="3" t="str">
-        <f t="shared" ref="D68:D69" si="1">IF(C68&lt;&gt;"",IF(B68&lt;&gt;"",B68-C68,"-"), "-")</f>
+        <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
@@ -1361,7 +1468,7 @@
       <c r="B69" s="5"/>
       <c r="C69" s="5"/>
       <c r="D69" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
@@ -1369,25 +1476,45 @@
       <c r="A70" s="5"/>
       <c r="B70" s="5"/>
       <c r="C70" s="5"/>
+      <c r="D70" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="71" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A71" s="5"/>
       <c r="B71" s="5"/>
       <c r="C71" s="5"/>
+      <c r="D71" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="72" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A72" s="5"/>
       <c r="B72" s="5"/>
       <c r="C72" s="5"/>
+      <c r="D72" s="3" t="str">
+        <f t="shared" ref="D72:D73" si="2">IF(C72&lt;&gt;"",IF(B72&lt;&gt;"",B72-C72,"-"), "-")</f>
+        <v>-</v>
+      </c>
     </row>
     <row r="73" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A73" s="5"/>
       <c r="B73" s="5"/>
       <c r="C73" s="5"/>
+      <c r="D73" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="74" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A74" s="5"/>
       <c r="B74" s="5"/>
       <c r="C74" s="5"/>
     </row>
     <row r="75" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A75" s="5"/>
       <c r="B75" s="5"/>
       <c r="C75" s="5"/>
     </row>
@@ -1922,6 +2049,22 @@
     <row r="208" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B208" s="5"/>
       <c r="C208" s="5"/>
+    </row>
+    <row r="209" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B209" s="5"/>
+      <c r="C209" s="5"/>
+    </row>
+    <row r="210" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B210" s="5"/>
+      <c r="C210" s="5"/>
+    </row>
+    <row r="211" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B211" s="5"/>
+      <c r="C211" s="5"/>
+    </row>
+    <row r="212" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B212" s="5"/>
+      <c r="C212" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
level 2 10 ahead
</commit_message>
<xml_diff>
--- a/GenesisMarbleMadness/FrameCompare.xlsx
+++ b/GenesisMarbleMadness/FrameCompare.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\GenesisMarbleMadness\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E09C3F4-53E8-4B83-8F35-EDBBA1E3BD0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CD5F89F-FE34-4B19-A2F9-C9B013A33238}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-7950" yWindow="300" windowWidth="7965" windowHeight="12825" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-6975" yWindow="300" windowWidth="6990" windowHeight="12825" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="V3" sheetId="7" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="48">
   <si>
     <t>Place</t>
   </si>
@@ -166,6 +166,15 @@
   </si>
   <si>
     <t>about to leap</t>
+  </si>
+  <si>
+    <t>Lv 2 Title Screen</t>
+  </si>
+  <si>
+    <t>crack enemy marble</t>
+  </si>
+  <si>
+    <t>flat ramp</t>
   </si>
 </sst>
 </file>
@@ -660,11 +669,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A88CD45-A2B6-49C4-A4B2-BB74C4A0A2BD}">
-  <dimension ref="A1:F212"/>
+  <dimension ref="A1:F215"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
+      <selection pane="bottomLeft" activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -697,7 +706,7 @@
         <v>427</v>
       </c>
       <c r="D2" s="3" t="str">
-        <f t="shared" ref="D2:D71" si="0">IF(C2&lt;&gt;"",IF(B2&lt;&gt;"",C2-B2,"-"), "-")</f>
+        <f t="shared" ref="D2:D74" si="0">IF(C2&lt;&gt;"",IF(B2&lt;&gt;"",C2-B2,"-"), "-")</f>
         <v>-</v>
       </c>
       <c r="F2" s="2"/>
@@ -735,7 +744,9 @@
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
-      <c r="F4" s="2"/>
+      <c r="E4" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
@@ -751,7 +762,9 @@
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="F5" s="2"/>
+      <c r="E5" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
@@ -767,7 +780,9 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="F6" s="2"/>
+      <c r="E6" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
@@ -783,7 +798,9 @@
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="F7" s="2"/>
+      <c r="E7" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
@@ -799,7 +816,9 @@
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="F8" s="2"/>
+      <c r="E8" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
@@ -815,7 +834,9 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="F9" s="2"/>
+      <c r="E9" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
@@ -831,7 +852,9 @@
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="F10" s="2"/>
+      <c r="E10" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
@@ -847,17 +870,13 @@
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="E11">
-        <f>C11-41</f>
-        <v>1052</v>
-      </c>
-      <c r="F11" t="s">
-        <v>33</v>
+      <c r="E11" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
-        <v>7</v>
+      <c r="A12" s="12" t="s">
+        <v>45</v>
       </c>
       <c r="B12" s="2">
         <v>1422</v>
@@ -869,273 +888,283 @@
         <f t="shared" ref="D12" si="1">IF(C12&lt;&gt;"",IF(B12&lt;&gt;"",C12-B12,"-"), "-")</f>
         <v>33</v>
       </c>
-      <c r="F12" t="s">
-        <v>34</v>
-      </c>
     </row>
     <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F13" t="s">
-        <v>35</v>
+      <c r="A13" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="2">
+        <v>1603</v>
+      </c>
+      <c r="C13" s="2">
+        <v>1636</v>
+      </c>
+      <c r="D13" s="3">
+        <f t="shared" si="0"/>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F14" t="s">
-        <v>36</v>
+      <c r="A14" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="2">
+        <v>1610</v>
+      </c>
+      <c r="C14" s="2">
+        <v>1641</v>
+      </c>
+      <c r="D14" s="3">
+        <f t="shared" si="0"/>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="3"/>
-      <c r="F15" t="s">
-        <v>37</v>
+      <c r="A15" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="2">
+        <v>1723</v>
+      </c>
+      <c r="C15" s="2">
+        <v>1744</v>
+      </c>
+      <c r="D15" s="3">
+        <f t="shared" si="0"/>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F16" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
-        <v>16</v>
-      </c>
+      <c r="A16" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="2">
+        <v>1762</v>
+      </c>
+      <c r="C16" s="2">
+        <v>1781</v>
+      </c>
+      <c r="D16" s="3">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A17" s="7"/>
       <c r="B17" s="2"/>
-      <c r="C17" s="2">
-        <v>1782</v>
-      </c>
+      <c r="C17" s="2"/>
       <c r="D17" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="F17" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="2"/>
+      <c r="B18" s="2">
+        <v>1963</v>
+      </c>
       <c r="C18" s="2">
-        <v>1980</v>
-      </c>
-      <c r="D18" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F18" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
+        <v>1981</v>
+      </c>
+      <c r="D18" s="3">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="2">
+        <v>2110</v>
+      </c>
+      <c r="C19" s="2">
+        <v>2121</v>
+      </c>
+      <c r="D19" s="3">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A20" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="2">
+        <v>2236</v>
+      </c>
+      <c r="C20" s="2">
+        <v>2248</v>
+      </c>
+      <c r="D20" s="3">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="2">
+        <v>2381</v>
+      </c>
+      <c r="C21" s="2">
+        <v>2391</v>
+      </c>
+      <c r="D21" s="3">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A22" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" s="2">
+        <v>2962</v>
+      </c>
+      <c r="C22" s="2">
+        <v>2972</v>
+      </c>
+      <c r="D22" s="3">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="2">
+        <v>2806</v>
+      </c>
+      <c r="C23" s="2">
+        <v>2816</v>
+      </c>
+      <c r="D23" s="3">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
         <v>15</v>
-      </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2">
-        <v>2128</v>
-      </c>
-      <c r="D19" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2">
-        <v>2816</v>
-      </c>
-      <c r="D20" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2">
-        <v>3449</v>
-      </c>
-      <c r="D21" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2">
-        <v>3894</v>
-      </c>
-      <c r="D22" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2">
-        <v>4014</v>
-      </c>
-      <c r="D23" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
-        <v>22</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2">
-        <v>4939</v>
+        <v>3449</v>
       </c>
       <c r="D24" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2">
-        <v>5218</v>
+        <v>3894</v>
       </c>
       <c r="D25" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2">
-        <v>5394</v>
+        <v>4014</v>
       </c>
       <c r="D26" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2">
-        <v>5540</v>
+        <v>4939</v>
       </c>
       <c r="D27" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2">
-        <v>5851</v>
+        <v>5218</v>
       </c>
       <c r="D28" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A29" s="8"/>
+    <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
+        <v>23</v>
+      </c>
       <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="3"/>
-    </row>
-    <row r="30" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A30" s="9" t="s">
-        <v>26</v>
+      <c r="C29" s="2">
+        <v>5394</v>
+      </c>
+      <c r="D29" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
+        <v>25</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="2">
-        <v>6894</v>
+        <v>5540</v>
       </c>
       <c r="D30" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A31" s="9" t="s">
-        <v>27</v>
+    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A31" s="8" t="s">
+        <v>24</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2">
-        <v>7722</v>
+        <v>5851</v>
       </c>
       <c r="D31" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A32" s="10" t="s">
-        <v>28</v>
-      </c>
+    <row r="32" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A32" s="8"/>
       <c r="B32" s="2"/>
-      <c r="C32" s="2">
-        <v>7822</v>
-      </c>
-      <c r="D32" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
+      <c r="C32" s="2"/>
+      <c r="D32" s="3"/>
     </row>
     <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A33" s="10" t="s">
-        <v>29</v>
+      <c r="A33" s="9" t="s">
+        <v>26</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2">
-        <v>7918</v>
+        <v>6894</v>
       </c>
       <c r="D33" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1143,49 +1172,61 @@
       </c>
     </row>
     <row r="34" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A34" s="6" t="s">
-        <v>6</v>
+      <c r="A34" s="9" t="s">
+        <v>27</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" s="2">
+        <v>7722</v>
+      </c>
+      <c r="D34" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A35" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2">
+        <v>7822</v>
+      </c>
+      <c r="D35" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A36" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2">
+        <v>7918</v>
+      </c>
+      <c r="D36" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A37" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2">
         <v>7924</v>
       </c>
-      <c r="D34" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
+      <c r="D37" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A36" s="5"/>
-      <c r="B36" s="5"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A37" s="5"/>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A38" s="5"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
       <c r="D38" s="3" t="str">
@@ -1495,7 +1536,7 @@
       <c r="B72" s="5"/>
       <c r="C72" s="5"/>
       <c r="D72" s="3" t="str">
-        <f t="shared" ref="D72:D73" si="2">IF(C72&lt;&gt;"",IF(B72&lt;&gt;"",B72-C72,"-"), "-")</f>
+        <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
@@ -1504,7 +1545,7 @@
       <c r="B73" s="5"/>
       <c r="C73" s="5"/>
       <c r="D73" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
@@ -1512,21 +1553,36 @@
       <c r="A74" s="5"/>
       <c r="B74" s="5"/>
       <c r="C74" s="5"/>
+      <c r="D74" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="75" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A75" s="5"/>
       <c r="B75" s="5"/>
       <c r="C75" s="5"/>
+      <c r="D75" s="3" t="str">
+        <f t="shared" ref="D75:D76" si="2">IF(C75&lt;&gt;"",IF(B75&lt;&gt;"",B75-C75,"-"), "-")</f>
+        <v>-</v>
+      </c>
     </row>
     <row r="76" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A76" s="5"/>
       <c r="B76" s="5"/>
       <c r="C76" s="5"/>
+      <c r="D76" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="77" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A77" s="5"/>
       <c r="B77" s="5"/>
       <c r="C77" s="5"/>
     </row>
     <row r="78" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A78" s="5"/>
       <c r="B78" s="5"/>
       <c r="C78" s="5"/>
     </row>
@@ -2065,6 +2121,18 @@
     <row r="212" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B212" s="5"/>
       <c r="C212" s="5"/>
+    </row>
+    <row r="213" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B213" s="5"/>
+      <c r="C213" s="5"/>
+    </row>
+    <row r="214" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B214" s="5"/>
+      <c r="C214" s="5"/>
+    </row>
+    <row r="215" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B215" s="5"/>
+      <c r="C215" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
mmv3 up to level 4
</commit_message>
<xml_diff>
--- a/GenesisMarbleMadness/FrameCompare.xlsx
+++ b/GenesisMarbleMadness/FrameCompare.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\GenesisMarbleMadness\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CD5F89F-FE34-4B19-A2F9-C9B013A33238}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37A4923E-E283-4061-91D9-FBE1788E9B6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-6975" yWindow="300" windowWidth="6990" windowHeight="12825" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="52">
   <si>
     <t>Place</t>
   </si>
@@ -175,6 +175,18 @@
   </si>
   <si>
     <t>flat ramp</t>
+  </si>
+  <si>
+    <t>Exit pipe (points)</t>
+  </si>
+  <si>
+    <t>enter pipe</t>
+  </si>
+  <si>
+    <t>Level 3 end (lag frame</t>
+  </si>
+  <si>
+    <t>first input frame</t>
   </si>
 </sst>
 </file>
@@ -669,11 +681,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A88CD45-A2B6-49C4-A4B2-BB74C4A0A2BD}">
-  <dimension ref="A1:F215"/>
+  <dimension ref="A1:F226"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C23" sqref="C23"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -706,7 +718,7 @@
         <v>427</v>
       </c>
       <c r="D2" s="3" t="str">
-        <f t="shared" ref="D2:D74" si="0">IF(C2&lt;&gt;"",IF(B2&lt;&gt;"",C2-B2,"-"), "-")</f>
+        <f t="shared" ref="D2:D85" si="0">IF(C2&lt;&gt;"",IF(B2&lt;&gt;"",C2-B2,"-"), "-")</f>
         <v>-</v>
       </c>
       <c r="F2" s="2"/>
@@ -977,15 +989,15 @@
       <c r="A19" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="2">
-        <v>2110</v>
+      <c r="B19" s="12">
+        <v>2099</v>
       </c>
       <c r="C19" s="2">
         <v>2121</v>
       </c>
       <c r="D19" s="3">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -993,14 +1005,14 @@
         <v>22</v>
       </c>
       <c r="B20" s="2">
-        <v>2236</v>
+        <v>2227</v>
       </c>
       <c r="C20" s="2">
         <v>2248</v>
       </c>
       <c r="D20" s="3">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -1008,324 +1020,392 @@
         <v>13</v>
       </c>
       <c r="B21" s="2">
-        <v>2381</v>
+        <v>2369</v>
       </c>
       <c r="C21" s="2">
         <v>2391</v>
       </c>
       <c r="D21" s="3">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" s="12" t="s">
+      <c r="A22" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" s="2">
+        <v>2794</v>
+      </c>
+      <c r="C22" s="2">
+        <v>2816</v>
+      </c>
+      <c r="D22" s="3">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B22" s="2">
-        <v>2962</v>
-      </c>
-      <c r="C22" s="2">
+      <c r="B23" s="2">
+        <v>2950</v>
+      </c>
+      <c r="C23" s="2">
         <v>2972</v>
       </c>
-      <c r="D22" s="3">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B23" s="2">
-        <v>2806</v>
-      </c>
-      <c r="C23" s="2">
-        <v>2816</v>
-      </c>
       <c r="D23" s="3">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B24" s="2"/>
+      <c r="A24" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="2">
+        <v>2955</v>
+      </c>
       <c r="C24" s="2">
+        <v>2979</v>
+      </c>
+      <c r="D24" s="3">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" s="12"/>
+      <c r="B25" s="2">
+        <v>2965</v>
+      </c>
+      <c r="C25" s="2">
+        <v>2991</v>
+      </c>
+      <c r="D25" s="3">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A26" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" s="2">
+        <v>2995</v>
+      </c>
+      <c r="C26" s="2">
+        <v>3015</v>
+      </c>
+      <c r="D26" s="3">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A27" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B27" s="2">
+        <v>3011</v>
+      </c>
+      <c r="C27" s="2">
+        <v>3031</v>
+      </c>
+      <c r="D27" s="3">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A28" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" s="2">
+        <v>3192</v>
+      </c>
+      <c r="C28" s="2">
+        <v>3216</v>
+      </c>
+      <c r="D28" s="3">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A29" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29" s="2">
+        <v>3259</v>
+      </c>
+      <c r="C29" s="2">
+        <v>3279</v>
+      </c>
+      <c r="D29" s="3">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A30" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B30" s="2">
+        <v>3365</v>
+      </c>
+      <c r="C30" s="2">
+        <v>3385</v>
+      </c>
+      <c r="D30" s="3">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A31" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B31" s="2">
+        <v>3429</v>
+      </c>
+      <c r="C31" s="2">
         <v>3449</v>
       </c>
-      <c r="D24" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="8" t="s">
+      <c r="D31" s="3">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A32" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32" s="2">
+        <v>3478</v>
+      </c>
+      <c r="C32" s="2">
+        <v>3494</v>
+      </c>
+      <c r="D32" s="3">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A33" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B33" s="2">
+        <v>3517</v>
+      </c>
+      <c r="C33" s="2">
+        <v>3533</v>
+      </c>
+      <c r="D33" s="3">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A34" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34" s="2">
+        <v>3647</v>
+      </c>
+      <c r="C34" s="2">
+        <v>3647</v>
+      </c>
+      <c r="D34" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A35" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B35" s="2">
+        <v>3656</v>
+      </c>
+      <c r="C35" s="2">
+        <v>3675</v>
+      </c>
+      <c r="D35" s="3">
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2">
-        <v>3894</v>
-      </c>
-      <c r="D25" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="s">
+    </row>
+    <row r="36" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="s">
         <v>20</v>
-      </c>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2">
-        <v>4014</v>
-      </c>
-      <c r="D26" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2">
-        <v>4939</v>
-      </c>
-      <c r="D27" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2">
-        <v>5218</v>
-      </c>
-      <c r="D28" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A29" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2">
-        <v>5394</v>
-      </c>
-      <c r="D29" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A30" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2">
-        <v>5540</v>
-      </c>
-      <c r="D30" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A31" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2">
-        <v>5851</v>
-      </c>
-      <c r="D31" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A32" s="8"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="3"/>
-    </row>
-    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A33" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2">
-        <v>6894</v>
-      </c>
-      <c r="D33" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A34" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2">
-        <v>7722</v>
-      </c>
-      <c r="D34" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A35" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2">
-        <v>7822</v>
-      </c>
-      <c r="D35" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A36" s="10" t="s">
-        <v>29</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" s="2">
+        <v>4014</v>
+      </c>
+      <c r="D36" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A37" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B37" s="2">
+        <v>4137</v>
+      </c>
+      <c r="C37" s="2">
+        <v>4155</v>
+      </c>
+      <c r="D37" s="3">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A38" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2">
+        <v>4939</v>
+      </c>
+      <c r="D38" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A39" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2">
+        <v>5218</v>
+      </c>
+      <c r="D39" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A40" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2">
+        <v>5394</v>
+      </c>
+      <c r="D40" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A41" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2">
+        <v>5540</v>
+      </c>
+      <c r="D41" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A42" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2">
+        <v>5851</v>
+      </c>
+      <c r="D42" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A43" s="8"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="3"/>
+    </row>
+    <row r="44" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A44" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2">
+        <v>6894</v>
+      </c>
+      <c r="D44" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A45" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2">
+        <v>7722</v>
+      </c>
+      <c r="D45" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A46" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2">
+        <v>7822</v>
+      </c>
+      <c r="D46" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A47" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2">
         <v>7918</v>
       </c>
-      <c r="D36" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A37" s="6" t="s">
+      <c r="D47" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A48" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2">
+      <c r="B48" s="2"/>
+      <c r="C48" s="2">
         <v>7924</v>
       </c>
-      <c r="D37" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
+      <c r="D48" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B38" s="5"/>
-      <c r="C38" s="5"/>
-      <c r="D38" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A39" s="5"/>
-      <c r="B39" s="5"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A40" s="5"/>
-      <c r="B40" s="5"/>
-      <c r="C40" s="5"/>
-      <c r="D40" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A41" s="5"/>
-      <c r="B41" s="5"/>
-      <c r="C41" s="5"/>
-      <c r="D41" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A42" s="5"/>
-      <c r="B42" s="5"/>
-      <c r="C42" s="5"/>
-      <c r="D42" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A43" s="5"/>
-      <c r="B43" s="5"/>
-      <c r="C43" s="5"/>
-      <c r="D43" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A44" s="5"/>
-      <c r="B44" s="5"/>
-      <c r="C44" s="5"/>
-      <c r="D44" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A45" s="5"/>
-      <c r="B45" s="5"/>
-      <c r="C45" s="5"/>
-      <c r="D45" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A46" s="5"/>
-      <c r="B46" s="5"/>
-      <c r="C46" s="5"/>
-      <c r="D46" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A47" s="5"/>
-      <c r="B47" s="5"/>
-      <c r="C47" s="5"/>
-      <c r="D47" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A48" s="5"/>
-      <c r="B48" s="5"/>
-      <c r="C48" s="5"/>
-      <c r="D48" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A49" s="5"/>
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
       <c r="D49" s="3" t="str">
@@ -1563,7 +1643,7 @@
       <c r="B75" s="5"/>
       <c r="C75" s="5"/>
       <c r="D75" s="3" t="str">
-        <f t="shared" ref="D75:D76" si="2">IF(C75&lt;&gt;"",IF(B75&lt;&gt;"",B75-C75,"-"), "-")</f>
+        <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
@@ -1572,7 +1652,7 @@
       <c r="B76" s="5"/>
       <c r="C76" s="5"/>
       <c r="D76" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
@@ -1580,81 +1660,136 @@
       <c r="A77" s="5"/>
       <c r="B77" s="5"/>
       <c r="C77" s="5"/>
+      <c r="D77" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="78" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A78" s="5"/>
       <c r="B78" s="5"/>
       <c r="C78" s="5"/>
+      <c r="D78" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="79" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A79" s="5"/>
       <c r="B79" s="5"/>
       <c r="C79" s="5"/>
+      <c r="D79" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="80" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A80" s="5"/>
       <c r="B80" s="5"/>
       <c r="C80" s="5"/>
-    </row>
-    <row r="81" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D80" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A81" s="5"/>
       <c r="B81" s="5"/>
       <c r="C81" s="5"/>
-    </row>
-    <row r="82" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D81" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A82" s="5"/>
       <c r="B82" s="5"/>
       <c r="C82" s="5"/>
-    </row>
-    <row r="83" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D82" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A83" s="5"/>
       <c r="B83" s="5"/>
       <c r="C83" s="5"/>
-    </row>
-    <row r="84" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D83" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A84" s="5"/>
       <c r="B84" s="5"/>
       <c r="C84" s="5"/>
-    </row>
-    <row r="85" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D84" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A85" s="5"/>
       <c r="B85" s="5"/>
       <c r="C85" s="5"/>
-    </row>
-    <row r="86" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D85" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A86" s="5"/>
       <c r="B86" s="5"/>
       <c r="C86" s="5"/>
-    </row>
-    <row r="87" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D86" s="3" t="str">
+        <f t="shared" ref="D86:D87" si="2">IF(C86&lt;&gt;"",IF(B86&lt;&gt;"",B86-C86,"-"), "-")</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A87" s="5"/>
       <c r="B87" s="5"/>
       <c r="C87" s="5"/>
-    </row>
-    <row r="88" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D87" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A88" s="5"/>
       <c r="B88" s="5"/>
       <c r="C88" s="5"/>
     </row>
-    <row r="89" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A89" s="5"/>
       <c r="B89" s="5"/>
       <c r="C89" s="5"/>
     </row>
-    <row r="90" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B90" s="5"/>
       <c r="C90" s="5"/>
     </row>
-    <row r="91" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B91" s="5"/>
       <c r="C91" s="5"/>
     </row>
-    <row r="92" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B92" s="5"/>
       <c r="C92" s="5"/>
     </row>
-    <row r="93" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B93" s="5"/>
       <c r="C93" s="5"/>
     </row>
-    <row r="94" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B94" s="5"/>
       <c r="C94" s="5"/>
     </row>
-    <row r="95" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B95" s="5"/>
       <c r="C95" s="5"/>
     </row>
-    <row r="96" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B96" s="5"/>
       <c r="C96" s="5"/>
     </row>
@@ -2133,6 +2268,50 @@
     <row r="215" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B215" s="5"/>
       <c r="C215" s="5"/>
+    </row>
+    <row r="216" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B216" s="5"/>
+      <c r="C216" s="5"/>
+    </row>
+    <row r="217" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B217" s="5"/>
+      <c r="C217" s="5"/>
+    </row>
+    <row r="218" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B218" s="5"/>
+      <c r="C218" s="5"/>
+    </row>
+    <row r="219" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B219" s="5"/>
+      <c r="C219" s="5"/>
+    </row>
+    <row r="220" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B220" s="5"/>
+      <c r="C220" s="5"/>
+    </row>
+    <row r="221" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B221" s="5"/>
+      <c r="C221" s="5"/>
+    </row>
+    <row r="222" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B222" s="5"/>
+      <c r="C222" s="5"/>
+    </row>
+    <row r="223" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B223" s="5"/>
+      <c r="C223" s="5"/>
+    </row>
+    <row r="224" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B224" s="5"/>
+      <c r="C224" s="5"/>
+    </row>
+    <row r="225" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B225" s="5"/>
+      <c r="C225" s="5"/>
+    </row>
+    <row r="226" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B226" s="5"/>
+      <c r="C226" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>